<commit_message>
Ui updated with authentication and modules working on user uploaded data
</commit_message>
<xml_diff>
--- a/Agile_document_crypto_manager_project.xlsx
+++ b/Agile_document_crypto_manager_project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priya\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B52534-F84E-4CAD-9C18-41D84330DCC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488C088F-4B23-4124-8474-E71EB7A39BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -360,7 +360,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="224">
   <si>
     <t>Planned Sprint</t>
   </si>
@@ -1020,6 +1020,24 @@
   <si>
     <t>applied stress test for sample data and checked whether the portfolio behaves with the market or not</t>
   </si>
+  <si>
+    <t>3rd Oct</t>
+  </si>
+  <si>
+    <t>4th Oct</t>
+  </si>
+  <si>
+    <t>Mock Presentation</t>
+  </si>
+  <si>
+    <t>6th Oct</t>
+  </si>
+  <si>
+    <t>Little change in stress test to simulate better</t>
+  </si>
+  <si>
+    <t>Better the presentation by explaining the project and not to go deep with the terminologies</t>
+  </si>
 </sst>
 </file>
 
@@ -1499,6 +1517,15 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1516,15 +1543,6 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1723,7 +1741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -3436,7 +3454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
@@ -3488,28 +3506,28 @@
       <c r="Z1" s="14"/>
     </row>
     <row r="2" spans="1:26" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="67" t="s">
+      <c r="C2" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="69" t="s">
+      <c r="E2" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="67" t="s">
+      <c r="F2" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="67" t="s">
+      <c r="G2" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="67" t="s">
+      <c r="H2" s="70" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="15" t="s">
@@ -3562,14 +3580,14 @@
       <c r="Z2" s="17"/>
     </row>
     <row r="3" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="66"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
+      <c r="A3" s="69"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
       <c r="I3" s="18">
         <f t="shared" ref="I3:W3" si="0">SUM(I5:I800)</f>
         <v>33</v>
@@ -3635,31 +3653,31 @@
       <c r="Z3" s="17"/>
     </row>
     <row r="4" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
-      <c r="M4" s="65"/>
-      <c r="N4" s="65"/>
-      <c r="O4" s="65"/>
-      <c r="P4" s="65"/>
-      <c r="Q4" s="65"/>
-      <c r="R4" s="65"/>
-      <c r="S4" s="65"/>
-      <c r="T4" s="65"/>
-      <c r="U4" s="65"/>
-      <c r="V4" s="65"/>
-      <c r="W4" s="65"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="68"/>
+      <c r="P4" s="68"/>
+      <c r="Q4" s="68"/>
+      <c r="R4" s="68"/>
+      <c r="S4" s="68"/>
+      <c r="T4" s="68"/>
+      <c r="U4" s="68"/>
+      <c r="V4" s="68"/>
+      <c r="W4" s="68"/>
       <c r="X4" s="17"/>
       <c r="Y4" s="17"/>
       <c r="Z4" s="17"/>
@@ -3955,31 +3973,31 @@
       <c r="Z10" s="14"/>
     </row>
     <row r="11" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="65"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="65"/>
-      <c r="N11" s="65"/>
-      <c r="O11" s="65"/>
-      <c r="P11" s="65"/>
-      <c r="Q11" s="65"/>
-      <c r="R11" s="65"/>
-      <c r="S11" s="65"/>
-      <c r="T11" s="65"/>
-      <c r="U11" s="65"/>
-      <c r="V11" s="65"/>
-      <c r="W11" s="65"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="68"/>
+      <c r="L11" s="68"/>
+      <c r="M11" s="68"/>
+      <c r="N11" s="68"/>
+      <c r="O11" s="68"/>
+      <c r="P11" s="68"/>
+      <c r="Q11" s="68"/>
+      <c r="R11" s="68"/>
+      <c r="S11" s="68"/>
+      <c r="T11" s="68"/>
+      <c r="U11" s="68"/>
+      <c r="V11" s="68"/>
+      <c r="W11" s="68"/>
       <c r="X11" s="14"/>
       <c r="Y11" s="14"/>
       <c r="Z11" s="14"/>
@@ -4277,31 +4295,31 @@
       <c r="Z17" s="14"/>
     </row>
     <row r="18" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="65" t="s">
+      <c r="A18" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="65"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="65"/>
-      <c r="J18" s="65"/>
-      <c r="K18" s="65"/>
-      <c r="L18" s="65"/>
-      <c r="M18" s="65"/>
-      <c r="N18" s="65"/>
-      <c r="O18" s="65"/>
-      <c r="P18" s="65"/>
-      <c r="Q18" s="65"/>
-      <c r="R18" s="65"/>
-      <c r="S18" s="65"/>
-      <c r="T18" s="65"/>
-      <c r="U18" s="65"/>
-      <c r="V18" s="65"/>
-      <c r="W18" s="65"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="68"/>
+      <c r="L18" s="68"/>
+      <c r="M18" s="68"/>
+      <c r="N18" s="68"/>
+      <c r="O18" s="68"/>
+      <c r="P18" s="68"/>
+      <c r="Q18" s="68"/>
+      <c r="R18" s="68"/>
+      <c r="S18" s="68"/>
+      <c r="T18" s="68"/>
+      <c r="U18" s="68"/>
+      <c r="V18" s="68"/>
+      <c r="W18" s="68"/>
       <c r="X18" s="14"/>
       <c r="Y18" s="14"/>
       <c r="Z18" s="14"/>
@@ -4553,31 +4571,31 @@
       <c r="Z23" s="14"/>
     </row>
     <row r="24" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="68" t="s">
         <v>125</v>
       </c>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="65"/>
-      <c r="M24" s="65"/>
-      <c r="N24" s="65"/>
-      <c r="O24" s="65"/>
-      <c r="P24" s="65"/>
-      <c r="Q24" s="65"/>
-      <c r="R24" s="65"/>
-      <c r="S24" s="65"/>
-      <c r="T24" s="65"/>
-      <c r="U24" s="65"/>
-      <c r="V24" s="65"/>
-      <c r="W24" s="65"/>
+      <c r="B24" s="68"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="68"/>
+      <c r="J24" s="68"/>
+      <c r="K24" s="68"/>
+      <c r="L24" s="68"/>
+      <c r="M24" s="68"/>
+      <c r="N24" s="68"/>
+      <c r="O24" s="68"/>
+      <c r="P24" s="68"/>
+      <c r="Q24" s="68"/>
+      <c r="R24" s="68"/>
+      <c r="S24" s="68"/>
+      <c r="T24" s="68"/>
+      <c r="U24" s="68"/>
+      <c r="V24" s="68"/>
+      <c r="W24" s="68"/>
       <c r="X24" s="14"/>
       <c r="Y24" s="14"/>
       <c r="Z24" s="14"/>
@@ -32003,8 +32021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G992"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="D43" sqref="D42:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -32041,10 +32059,10 @@
       <c r="B2" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="65" t="s">
         <v>151</v>
       </c>
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="65" t="s">
         <v>188</v>
       </c>
       <c r="E2" s="50"/>
@@ -32056,10 +32074,10 @@
       <c r="B3" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="65" t="s">
         <v>152</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="D3" s="65" t="s">
         <v>190</v>
       </c>
     </row>
@@ -32070,10 +32088,10 @@
       <c r="B4" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="C4" s="71" t="s">
+      <c r="C4" s="65" t="s">
         <v>154</v>
       </c>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="65" t="s">
         <v>187</v>
       </c>
     </row>
@@ -32084,10 +32102,10 @@
       <c r="B5" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="C5" s="72" t="s">
+      <c r="C5" s="66" t="s">
         <v>153</v>
       </c>
-      <c r="D5" s="72" t="s">
+      <c r="D5" s="66" t="s">
         <v>189</v>
       </c>
     </row>
@@ -32098,10 +32116,10 @@
       <c r="B6" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="C6" s="71" t="s">
+      <c r="C6" s="65" t="s">
         <v>155</v>
       </c>
-      <c r="D6" s="71" t="s">
+      <c r="D6" s="65" t="s">
         <v>191</v>
       </c>
     </row>
@@ -32112,10 +32130,10 @@
       <c r="B7" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="C7" s="72" t="s">
+      <c r="C7" s="66" t="s">
         <v>156</v>
       </c>
-      <c r="D7" s="72" t="s">
+      <c r="D7" s="66" t="s">
         <v>192</v>
       </c>
     </row>
@@ -32126,10 +32144,10 @@
       <c r="B8" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="C8" s="71" t="s">
+      <c r="C8" s="65" t="s">
         <v>157</v>
       </c>
-      <c r="D8" s="71" t="s">
+      <c r="D8" s="65" t="s">
         <v>193</v>
       </c>
     </row>
@@ -32140,10 +32158,10 @@
       <c r="B9" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="C9" s="71" t="s">
+      <c r="C9" s="65" t="s">
         <v>196</v>
       </c>
-      <c r="D9" s="71" t="s">
+      <c r="D9" s="65" t="s">
         <v>197</v>
       </c>
     </row>
@@ -32154,10 +32172,10 @@
       <c r="B10" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="C10" s="71" t="s">
+      <c r="C10" s="65" t="s">
         <v>158</v>
       </c>
-      <c r="D10" s="71" t="s">
+      <c r="D10" s="65" t="s">
         <v>194</v>
       </c>
     </row>
@@ -32168,7 +32186,7 @@
       <c r="B11" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="C11" s="71" t="s">
+      <c r="C11" s="65" t="s">
         <v>159</v>
       </c>
       <c r="D11" s="54" t="s">
@@ -32182,7 +32200,7 @@
       <c r="B12" s="52" t="s">
         <v>150</v>
       </c>
-      <c r="C12" s="71" t="s">
+      <c r="C12" s="65" t="s">
         <v>160</v>
       </c>
       <c r="D12" s="54" t="s">
@@ -32196,10 +32214,10 @@
       <c r="B13" s="52" t="s">
         <v>161</v>
       </c>
-      <c r="C13" s="71" t="s">
+      <c r="C13" s="65" t="s">
         <v>162</v>
       </c>
-      <c r="D13" s="71" t="s">
+      <c r="D13" s="65" t="s">
         <v>195</v>
       </c>
     </row>
@@ -32210,10 +32228,10 @@
       <c r="B14" s="52" t="s">
         <v>163</v>
       </c>
-      <c r="C14" s="71" t="s">
+      <c r="C14" s="65" t="s">
         <v>178</v>
       </c>
-      <c r="D14" s="71" t="s">
+      <c r="D14" s="65" t="s">
         <v>198</v>
       </c>
     </row>
@@ -32224,10 +32242,10 @@
       <c r="B15" s="52" t="s">
         <v>164</v>
       </c>
-      <c r="C15" s="71" t="s">
+      <c r="C15" s="65" t="s">
         <v>184</v>
       </c>
-      <c r="D15" s="71" t="s">
+      <c r="D15" s="65" t="s">
         <v>199</v>
       </c>
     </row>
@@ -32238,10 +32256,10 @@
       <c r="B16" s="52" t="s">
         <v>165</v>
       </c>
-      <c r="C16" s="71" t="s">
+      <c r="C16" s="65" t="s">
         <v>179</v>
       </c>
-      <c r="D16" s="71" t="s">
+      <c r="D16" s="65" t="s">
         <v>200</v>
       </c>
     </row>
@@ -32252,10 +32270,10 @@
       <c r="B17" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="C17" s="71" t="s">
+      <c r="C17" s="65" t="s">
         <v>180</v>
       </c>
-      <c r="D17" s="71" t="s">
+      <c r="D17" s="65" t="s">
         <v>201</v>
       </c>
     </row>
@@ -32266,10 +32284,10 @@
       <c r="B18" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="C18" s="71" t="s">
+      <c r="C18" s="65" t="s">
         <v>203</v>
       </c>
-      <c r="D18" s="71" t="s">
+      <c r="D18" s="65" t="s">
         <v>202</v>
       </c>
     </row>
@@ -32280,10 +32298,10 @@
       <c r="B19" s="52" t="s">
         <v>168</v>
       </c>
-      <c r="C19" s="71" t="s">
+      <c r="C19" s="65" t="s">
         <v>158</v>
       </c>
-      <c r="D19" s="71" t="s">
+      <c r="D19" s="65" t="s">
         <v>204</v>
       </c>
     </row>
@@ -32294,7 +32312,7 @@
       <c r="B20" s="52" t="s">
         <v>169</v>
       </c>
-      <c r="C20" s="71" t="s">
+      <c r="C20" s="65" t="s">
         <v>158</v>
       </c>
       <c r="D20" s="54" t="s">
@@ -32308,7 +32326,7 @@
       <c r="B21" s="52" t="s">
         <v>170</v>
       </c>
-      <c r="C21" s="71" t="s">
+      <c r="C21" s="65" t="s">
         <v>181</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -32322,7 +32340,7 @@
       <c r="B22" s="52" t="s">
         <v>171</v>
       </c>
-      <c r="C22" s="71" t="s">
+      <c r="C22" s="65" t="s">
         <v>182</v>
       </c>
       <c r="D22" s="3" t="s">
@@ -32336,10 +32354,10 @@
       <c r="B23" s="52" t="s">
         <v>172</v>
       </c>
-      <c r="C23" s="71" t="s">
+      <c r="C23" s="65" t="s">
         <v>183</v>
       </c>
-      <c r="D23" s="71" t="s">
+      <c r="D23" s="65" t="s">
         <v>207</v>
       </c>
     </row>
@@ -32350,10 +32368,10 @@
       <c r="B24" s="52" t="s">
         <v>173</v>
       </c>
-      <c r="C24" s="71" t="s">
+      <c r="C24" s="65" t="s">
         <v>185</v>
       </c>
-      <c r="D24" s="71" t="s">
+      <c r="D24" s="65" t="s">
         <v>208</v>
       </c>
     </row>
@@ -32364,7 +32382,7 @@
       <c r="B25" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="C25" s="71" t="s">
+      <c r="C25" s="65" t="s">
         <v>186</v>
       </c>
       <c r="D25" s="3" t="s">
@@ -32378,10 +32396,10 @@
       <c r="B26" s="52" t="s">
         <v>175</v>
       </c>
-      <c r="C26" s="71" t="s">
+      <c r="C26" s="65" t="s">
         <v>158</v>
       </c>
-      <c r="D26" s="71" t="s">
+      <c r="D26" s="65" t="s">
         <v>210</v>
       </c>
     </row>
@@ -32392,10 +32410,10 @@
       <c r="B27" s="52" t="s">
         <v>176</v>
       </c>
-      <c r="C27" s="71" t="s">
+      <c r="C27" s="65" t="s">
         <v>158</v>
       </c>
-      <c r="D27" s="71" t="s">
+      <c r="D27" s="65" t="s">
         <v>211</v>
       </c>
     </row>
@@ -32406,7 +32424,7 @@
       <c r="B28" s="52" t="s">
         <v>177</v>
       </c>
-      <c r="C28" s="71" t="s">
+      <c r="C28" s="65" t="s">
         <v>158</v>
       </c>
       <c r="D28" s="54" t="s">
@@ -32420,10 +32438,10 @@
       <c r="B29" s="52" t="s">
         <v>212</v>
       </c>
-      <c r="C29" s="71" t="s">
+      <c r="C29" s="65" t="s">
         <v>214</v>
       </c>
-      <c r="D29" s="73" t="s">
+      <c r="D29" s="67" t="s">
         <v>215</v>
       </c>
     </row>
@@ -32434,31 +32452,70 @@
       <c r="B30" s="52" t="s">
         <v>213</v>
       </c>
-      <c r="C30" s="71" t="s">
+      <c r="C30" s="65" t="s">
         <v>216</v>
       </c>
-      <c r="D30" s="71" t="s">
+      <c r="D30" s="65" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="24">
+        <v>4</v>
+      </c>
+      <c r="B31" s="52" t="s">
+        <v>218</v>
+      </c>
+      <c r="C31" s="65" t="s">
+        <v>158</v>
+      </c>
+      <c r="D31" s="65" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="24">
+        <v>4</v>
+      </c>
+      <c r="B32" s="52" t="s">
+        <v>219</v>
+      </c>
+      <c r="C32" s="65" t="s">
+        <v>158</v>
+      </c>
+      <c r="D32" s="54" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="24">
+        <v>4</v>
+      </c>
+      <c r="B33" s="52" t="s">
+        <v>221</v>
+      </c>
+      <c r="C33" s="65" t="s">
+        <v>220</v>
+      </c>
+      <c r="D33" s="65" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -33414,7 +33471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changes made to the authentication
</commit_message>
<xml_diff>
--- a/Agile_document_crypto_manager_project.xlsx
+++ b/Agile_document_crypto_manager_project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priya\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488C088F-4B23-4124-8474-E71EB7A39BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C07666-074E-4F28-9327-C6E8CCA07BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -1741,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -33471,7 +33471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>